<commit_message>
added flowchart for knn
</commit_message>
<xml_diff>
--- a/analysis/results.xlsx
+++ b/analysis/results.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonge/Documents/Classes/CS182/project/chameleon-mouth/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Frank's JetDrive Lite 330/Google Drive/Frank/University/Semester 7/CS 182/chameleon-mouth/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27960" windowHeight="23120" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="KNN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Obama</t>
   </si>
@@ -57,12 +58,27 @@
   </si>
   <si>
     <t>Avg Length of Word</t>
+  </si>
+  <si>
+    <t>Length of tweet</t>
+  </si>
+  <si>
+    <t>Number of hashtags</t>
+  </si>
+  <si>
+    <t>Number of links</t>
+  </si>
+  <si>
+    <t>Number of mentions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -100,10 +116,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
@@ -627,4 +645,224 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.68969999999999998</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.68630000000000002</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.62409999999999999</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.66600000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.62070000000000003</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.72550000000000003</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.6069</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.66200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.4098</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.4138</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.51959999999999995</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.1966</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.80889999999999995</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>0.74880000000000002</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.251193</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.72409999999999997</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.755</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.61029999999999995</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.67800000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>